<commit_message>
Update with Microsoft Nodes
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/CPU/report_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/CPU/report_CPUExecutionProvider.xlsx
@@ -27,7 +27,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -37,19 +37,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0000AA44"/>
-        <bgColor rgb="0000AA44"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00007700"/>
-        <bgColor rgb="00007700"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00DEDEDE"/>
-        <bgColor rgb="00DEDEDE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004D7CFE"/>
       </patternFill>
     </fill>
   </fills>
@@ -62,29 +64,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -178,7 +173,6 @@
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
       <pieChart>
@@ -250,6 +244,28 @@
             <idx val="5"/>
             <spPr>
               <a:solidFill>
+                <a:srgbClr val="4D7CFE"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="6"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="7"/>
+            <spPr>
+              <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
@@ -259,12 +275,12 @@
           </dPt>
           <cat>
             <numRef>
-              <f>'Data_PieChart'!$A$2:$A$7</f>
+              <f>'Data_PieChart'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Data_PieChart'!$B$2:$B$7</f>
+              <f>'Data_PieChart'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -599,7 +615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,10 +623,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="48" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="29" customWidth="1" min="4" max="4"/>
+    <col width="80" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -660,7 +676,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Div</t>
+          <t>AffineGrid</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -682,7 +698,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Sub</t>
+          <t>And</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
@@ -704,7 +720,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Mul</t>
+          <t>ArgMax</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -726,7 +742,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Pow</t>
+          <t>ArgMin</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
@@ -748,7 +764,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Mod</t>
+          <t>AveragePool</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -770,7 +786,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>BitwiseAnd</t>
+          <t>BatchNormalization</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -792,7 +808,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>BitwiseOr</t>
+          <t>Bernoulli</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
@@ -807,14 +823,14 @@
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>BitwiseXor</t>
+          <t>BitShift</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
@@ -836,7 +852,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>And</t>
+          <t>BitwiseAnd</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
@@ -858,7 +874,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Or</t>
+          <t>BitwiseNot</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
@@ -880,7 +896,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Xor</t>
+          <t>BitwiseOr</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
@@ -902,7 +918,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>ReduceSum</t>
+          <t>BitwiseXor</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -924,7 +940,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>ReduceMean</t>
+          <t>BlackmanWindow</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
@@ -946,7 +962,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>ReduceMax</t>
+          <t>Cast</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
@@ -968,7 +984,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>ReduceMin</t>
+          <t>CastLike</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -983,14 +999,14 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>ReduceProd</t>
+          <t>CenterCropPad</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
@@ -1005,14 +1021,14 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>ReduceL1</t>
+          <t>Clip</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
@@ -1034,7 +1050,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>ReduceL2</t>
+          <t>Col2Im</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
@@ -1056,7 +1072,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>ReduceLogSum</t>
+          <t>Compress</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
@@ -1078,7 +1094,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>ReduceLogSumExp</t>
+          <t>Concat</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
@@ -1100,7 +1116,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>ReduceSumSquare</t>
+          <t>ConcatFromSequence</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
@@ -1122,7 +1138,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Equal</t>
+          <t>Constant</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
@@ -1130,21 +1146,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D24" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C24" s="1" t="inlineStr"/>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>UNKNOWN (no Node event)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Not</t>
+          <t>ConstantOfShape</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
@@ -1166,7 +1178,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Greater</t>
+          <t>Conv</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
@@ -1188,7 +1200,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Less</t>
+          <t>ConvInteger</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
@@ -1210,7 +1222,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>GreaterOrEqual</t>
+          <t>ConvTranspose</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
@@ -1232,7 +1244,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>LessOrEqual</t>
+          <t>CumSum</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
@@ -1254,7 +1266,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Not</t>
+          <t>DFT</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
@@ -1276,7 +1288,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>IsNaN</t>
+          <t>DeformConv</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
@@ -1284,21 +1296,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C31" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C31" s="1" t="inlineStr"/>
+      <c r="D31" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DeformConv(19) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>IsInf</t>
+          <t>DepthToSpace</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
@@ -1320,7 +1328,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>DequantizeLinear</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
@@ -1342,7 +1350,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Min</t>
+          <t>Det</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
@@ -1364,7 +1372,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Mean</t>
+          <t>Div</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
@@ -1386,7 +1394,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Sum</t>
+          <t>Dropout</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
@@ -1408,7 +1416,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>ArgMin</t>
+          <t>DynamicQuantizeLinear</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
@@ -1430,7 +1438,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>ArgMax</t>
+          <t>Einsum</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
@@ -1452,7 +1460,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Reshape</t>
+          <t>Equal</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr">
@@ -1496,7 +1504,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Flatten</t>
+          <t>EyeLike</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr">
@@ -1518,7 +1526,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Squeeze</t>
+          <t>Flatten</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr">
@@ -1540,7 +1548,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Unsqueeze</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B43" s="1" t="inlineStr">
@@ -1562,7 +1570,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Transpose</t>
+          <t>Gather</t>
         </is>
       </c>
       <c r="B44" s="1" t="inlineStr">
@@ -1584,7 +1592,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Concat</t>
+          <t>GatherElements</t>
         </is>
       </c>
       <c r="B45" s="1" t="inlineStr">
@@ -1606,7 +1614,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Split</t>
+          <t>GatherND</t>
         </is>
       </c>
       <c r="B46" s="1" t="inlineStr">
@@ -1628,7 +1636,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Slice</t>
+          <t>Gelu</t>
         </is>
       </c>
       <c r="B47" s="1" t="inlineStr">
@@ -1650,7 +1658,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Pad</t>
+          <t>Gemm</t>
         </is>
       </c>
       <c r="B48" s="1" t="inlineStr">
@@ -1672,7 +1680,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Tile</t>
+          <t>GlobalAveragePool</t>
         </is>
       </c>
       <c r="B49" s="1" t="inlineStr">
@@ -1694,7 +1702,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Gather</t>
+          <t>GlobalMaxPool</t>
         </is>
       </c>
       <c r="B50" s="1" t="inlineStr">
@@ -1716,7 +1724,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>GatherND</t>
+          <t>Greater</t>
         </is>
       </c>
       <c r="B51" s="1" t="inlineStr">
@@ -1738,7 +1746,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>GatherElements</t>
+          <t>GreaterOrEqual</t>
         </is>
       </c>
       <c r="B52" s="1" t="inlineStr">
@@ -1760,7 +1768,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>ScatterElements</t>
+          <t>GridSample</t>
         </is>
       </c>
       <c r="B53" s="1" t="inlineStr">
@@ -1782,7 +1790,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>ScatterND</t>
+          <t>GroupNormalization</t>
         </is>
       </c>
       <c r="B54" s="1" t="inlineStr">
@@ -1797,14 +1805,14 @@
       </c>
       <c r="D54" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Gemm</t>
+          <t>HammingWindow</t>
         </is>
       </c>
       <c r="B55" s="1" t="inlineStr">
@@ -1826,7 +1834,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>MatMul</t>
+          <t>HannWindow</t>
         </is>
       </c>
       <c r="B56" s="1" t="inlineStr">
@@ -1848,7 +1856,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>AveragePool</t>
+          <t>HardSigmoid</t>
         </is>
       </c>
       <c r="B57" s="1" t="inlineStr">
@@ -1870,7 +1878,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>MaxPool</t>
+          <t>HardSwish</t>
         </is>
       </c>
       <c r="B58" s="1" t="inlineStr">
@@ -1885,14 +1893,14 @@
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>GlobalMaxPool</t>
+          <t>Hardmax</t>
         </is>
       </c>
       <c r="B59" s="1" t="inlineStr">
@@ -1914,7 +1922,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>GlobalAveragePool</t>
+          <t>Identity</t>
         </is>
       </c>
       <c r="B60" s="1" t="inlineStr">
@@ -1936,7 +1944,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Dropout</t>
+          <t>If</t>
         </is>
       </c>
       <c r="B61" s="1" t="inlineStr">
@@ -1958,7 +1966,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>BatchNormalization</t>
+          <t>ImageDecoder</t>
         </is>
       </c>
       <c r="B62" s="1" t="inlineStr">
@@ -1966,14 +1974,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C62" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D62" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C62" s="1" t="inlineStr"/>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ImageDecoder(20) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2006,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>LayerNormalization</t>
+          <t>IsInf</t>
         </is>
       </c>
       <c r="B64" s="1" t="inlineStr">
@@ -2024,7 +2028,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>GroupNormalization</t>
+          <t>IsNaN</t>
         </is>
       </c>
       <c r="B65" s="1" t="inlineStr">
@@ -2037,16 +2041,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D65" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>AffineGrid</t>
+          <t>LRN</t>
         </is>
       </c>
       <c r="B66" s="1" t="inlineStr">
@@ -2068,7 +2072,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>GridSample</t>
+          <t>LSTM</t>
         </is>
       </c>
       <c r="B67" s="1" t="inlineStr">
@@ -2090,7 +2094,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Resize</t>
+          <t>LayerNormalization</t>
         </is>
       </c>
       <c r="B68" s="1" t="inlineStr">
@@ -2112,7 +2116,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Bernoulli</t>
+          <t>Less</t>
         </is>
       </c>
       <c r="B69" s="1" t="inlineStr">
@@ -2125,16 +2129,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D69" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>BitShift</t>
+          <t>LessOrEqual</t>
         </is>
       </c>
       <c r="B70" s="1" t="inlineStr">
@@ -2156,7 +2160,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>BitwiseNot</t>
+          <t>Loop</t>
         </is>
       </c>
       <c r="B71" s="1" t="inlineStr">
@@ -2178,7 +2182,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>BlackmanWindow</t>
+          <t>LpNormalization</t>
         </is>
       </c>
       <c r="B72" s="1" t="inlineStr">
@@ -2200,7 +2204,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>Cast</t>
+          <t>LpPool</t>
         </is>
       </c>
       <c r="B73" s="1" t="inlineStr">
@@ -2222,7 +2226,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>CastLike</t>
+          <t>MatMul</t>
         </is>
       </c>
       <c r="B74" s="1" t="inlineStr">
@@ -2235,16 +2239,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D74" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>CenterCropPad</t>
+          <t>MatMulInteger</t>
         </is>
       </c>
       <c r="B75" s="1" t="inlineStr">
@@ -2257,16 +2261,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D75" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>Clip</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="B76" s="1" t="inlineStr">
@@ -2288,7 +2292,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>Col2Im</t>
+          <t>MaxPool</t>
         </is>
       </c>
       <c r="B77" s="1" t="inlineStr">
@@ -2310,7 +2314,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>Compress</t>
+          <t>MaxRoiPool</t>
         </is>
       </c>
       <c r="B78" s="1" t="inlineStr">
@@ -2332,7 +2336,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>ConcatFromSequence</t>
+          <t>MaxUnpool</t>
         </is>
       </c>
       <c r="B79" s="1" t="inlineStr">
@@ -2354,7 +2358,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>Constant</t>
+          <t>Mean</t>
         </is>
       </c>
       <c r="B80" s="1" t="inlineStr">
@@ -2362,17 +2366,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C80" s="1" t="inlineStr"/>
-      <c r="D80" s="4" t="inlineStr">
-        <is>
-          <t>UNKNOWN (no Node event)</t>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>ConstantOfShape</t>
+          <t>MeanVarianceNormalization</t>
         </is>
       </c>
       <c r="B81" s="1" t="inlineStr">
@@ -2394,7 +2402,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>Conv</t>
+          <t>MelWeightMatrix</t>
         </is>
       </c>
       <c r="B82" s="1" t="inlineStr">
@@ -2416,7 +2424,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>ConvTranspose</t>
+          <t>Min</t>
         </is>
       </c>
       <c r="B83" s="1" t="inlineStr">
@@ -2438,7 +2446,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>ConvInteger</t>
+          <t>Mod</t>
         </is>
       </c>
       <c r="B84" s="1" t="inlineStr">
@@ -2460,7 +2468,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>CumSum</t>
+          <t>Mul</t>
         </is>
       </c>
       <c r="B85" s="1" t="inlineStr">
@@ -2482,7 +2490,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>DFT</t>
+          <t>Multinomial</t>
         </is>
       </c>
       <c r="B86" s="1" t="inlineStr">
@@ -2504,7 +2512,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>DepthToSpace</t>
+          <t>NegativeLogLikelihoodLoss</t>
         </is>
       </c>
       <c r="B87" s="1" t="inlineStr">
@@ -2519,14 +2527,14 @@
       </c>
       <c r="D87" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>DequantizeLinear</t>
+          <t>NonMaxSuppression</t>
         </is>
       </c>
       <c r="B88" s="1" t="inlineStr">
@@ -2548,7 +2556,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>Det</t>
+          <t>NonZero</t>
         </is>
       </c>
       <c r="B89" s="1" t="inlineStr">
@@ -2570,7 +2578,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>DynamicQuantizeLinear</t>
+          <t>Not</t>
         </is>
       </c>
       <c r="B90" s="1" t="inlineStr">
@@ -2592,7 +2600,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>Einsum</t>
+          <t>Not</t>
         </is>
       </c>
       <c r="B91" s="1" t="inlineStr">
@@ -2614,7 +2622,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>EyeLike</t>
+          <t>OneHot</t>
         </is>
       </c>
       <c r="B92" s="1" t="inlineStr">
@@ -2636,7 +2644,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>Optional</t>
         </is>
       </c>
       <c r="B93" s="1" t="inlineStr">
@@ -2658,7 +2666,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>Gelu</t>
+          <t>OptionalGetElement</t>
         </is>
       </c>
       <c r="B94" s="1" t="inlineStr">
@@ -2680,7 +2688,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>HammingWindow</t>
+          <t>OptionalHasElement</t>
         </is>
       </c>
       <c r="B95" s="1" t="inlineStr">
@@ -2702,7 +2710,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>HannWindow</t>
+          <t>Or</t>
         </is>
       </c>
       <c r="B96" s="1" t="inlineStr">
@@ -2724,7 +2732,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>HardSigmoid</t>
+          <t>PRelu</t>
         </is>
       </c>
       <c r="B97" s="1" t="inlineStr">
@@ -2746,7 +2754,7 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>HardSwish</t>
+          <t>Pad</t>
         </is>
       </c>
       <c r="B98" s="1" t="inlineStr">
@@ -2759,16 +2767,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D98" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>Hardmax</t>
+          <t>Pow</t>
         </is>
       </c>
       <c r="B99" s="1" t="inlineStr">
@@ -2790,7 +2798,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>Identity</t>
+          <t>QLinearConv</t>
         </is>
       </c>
       <c r="B100" s="1" t="inlineStr">
@@ -2812,7 +2820,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>If</t>
+          <t>QLinearMatMul</t>
         </is>
       </c>
       <c r="B101" s="1" t="inlineStr">
@@ -2834,7 +2842,7 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>LRN</t>
+          <t>QuantizeLinear</t>
         </is>
       </c>
       <c r="B102" s="1" t="inlineStr">
@@ -2856,7 +2864,7 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>LSTM</t>
+          <t>RNN</t>
         </is>
       </c>
       <c r="B103" s="1" t="inlineStr">
@@ -2878,7 +2886,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>Loop</t>
+          <t>RandomNormal</t>
         </is>
       </c>
       <c r="B104" s="1" t="inlineStr">
@@ -2900,7 +2908,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>LpNormalization</t>
+          <t>RandomNormalLike</t>
         </is>
       </c>
       <c r="B105" s="1" t="inlineStr">
@@ -2922,7 +2930,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>LpPool</t>
+          <t>RandomUniform</t>
         </is>
       </c>
       <c r="B106" s="1" t="inlineStr">
@@ -2944,7 +2952,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>MatMulInteger</t>
+          <t>RandomUniformLike</t>
         </is>
       </c>
       <c r="B107" s="1" t="inlineStr">
@@ -2966,7 +2974,7 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>MaxRoiPool</t>
+          <t>Range</t>
         </is>
       </c>
       <c r="B108" s="1" t="inlineStr">
@@ -2988,7 +2996,7 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>MaxUnpool</t>
+          <t>ReduceL1</t>
         </is>
       </c>
       <c r="B109" s="1" t="inlineStr">
@@ -3010,7 +3018,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>MeanVarianceNormalization</t>
+          <t>ReduceL2</t>
         </is>
       </c>
       <c r="B110" s="1" t="inlineStr">
@@ -3032,7 +3040,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>MelWeightMatrix</t>
+          <t>ReduceLogSum</t>
         </is>
       </c>
       <c r="B111" s="1" t="inlineStr">
@@ -3054,7 +3062,7 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>Multinomial</t>
+          <t>ReduceLogSumExp</t>
         </is>
       </c>
       <c r="B112" s="1" t="inlineStr">
@@ -3076,7 +3084,7 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>NegativeLogLikelihoodLoss</t>
+          <t>ReduceMax</t>
         </is>
       </c>
       <c r="B113" s="1" t="inlineStr">
@@ -3089,16 +3097,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D113" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D113" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>NonMaxSuppression</t>
+          <t>ReduceMean</t>
         </is>
       </c>
       <c r="B114" s="1" t="inlineStr">
@@ -3120,7 +3128,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>NonZero</t>
+          <t>ReduceMin</t>
         </is>
       </c>
       <c r="B115" s="1" t="inlineStr">
@@ -3142,7 +3150,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>OneHot</t>
+          <t>ReduceProd</t>
         </is>
       </c>
       <c r="B116" s="1" t="inlineStr">
@@ -3164,7 +3172,7 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>Optional</t>
+          <t>ReduceSum</t>
         </is>
       </c>
       <c r="B117" s="1" t="inlineStr">
@@ -3186,7 +3194,7 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>OptionalGetElement</t>
+          <t>ReduceSumSquare</t>
         </is>
       </c>
       <c r="B118" s="1" t="inlineStr">
@@ -3208,7 +3216,7 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>OptionalHasElement</t>
+          <t>RegexFullMatch</t>
         </is>
       </c>
       <c r="B119" s="1" t="inlineStr">
@@ -3230,7 +3238,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>PRelu</t>
+          <t>Reshape</t>
         </is>
       </c>
       <c r="B120" s="1" t="inlineStr">
@@ -3252,7 +3260,7 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>QLinearConv</t>
+          <t>Resize</t>
         </is>
       </c>
       <c r="B121" s="1" t="inlineStr">
@@ -3274,7 +3282,7 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>QLinearMatMul</t>
+          <t>ReverseSequence</t>
         </is>
       </c>
       <c r="B122" s="1" t="inlineStr">
@@ -3296,7 +3304,7 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>QuantizeLinear</t>
+          <t>RoiAlign</t>
         </is>
       </c>
       <c r="B123" s="1" t="inlineStr">
@@ -3318,7 +3326,7 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>RNN</t>
+          <t>STFT</t>
         </is>
       </c>
       <c r="B124" s="1" t="inlineStr">
@@ -3340,7 +3348,7 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>RandomNormal</t>
+          <t>Scan</t>
         </is>
       </c>
       <c r="B125" s="1" t="inlineStr">
@@ -3362,7 +3370,7 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>RandomNormalLike</t>
+          <t>ScatterElements</t>
         </is>
       </c>
       <c r="B126" s="1" t="inlineStr">
@@ -3384,7 +3392,7 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>RandomUniform</t>
+          <t>ScatterND</t>
         </is>
       </c>
       <c r="B127" s="1" t="inlineStr">
@@ -3406,7 +3414,7 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>RandomUniformLike</t>
+          <t>SequenceAt</t>
         </is>
       </c>
       <c r="B128" s="1" t="inlineStr">
@@ -3428,7 +3436,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>Range</t>
+          <t>SequenceConstruct</t>
         </is>
       </c>
       <c r="B129" s="1" t="inlineStr">
@@ -3450,7 +3458,7 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>RegexFullMatch</t>
+          <t>SequenceEmpty</t>
         </is>
       </c>
       <c r="B130" s="1" t="inlineStr">
@@ -3472,7 +3480,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>ReverseSequence</t>
+          <t>SequenceErase</t>
         </is>
       </c>
       <c r="B131" s="1" t="inlineStr">
@@ -3494,7 +3502,7 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>RoiAlign</t>
+          <t>SequenceInsert</t>
         </is>
       </c>
       <c r="B132" s="1" t="inlineStr">
@@ -3516,7 +3524,7 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>STFT</t>
+          <t>SequenceLength</t>
         </is>
       </c>
       <c r="B133" s="1" t="inlineStr">
@@ -3538,7 +3546,7 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>Scan</t>
+          <t>SequenceMap</t>
         </is>
       </c>
       <c r="B134" s="1" t="inlineStr">
@@ -3553,14 +3561,14 @@
       </c>
       <c r="D134" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>SequenceAt</t>
+          <t>Shape</t>
         </is>
       </c>
       <c r="B135" s="1" t="inlineStr">
@@ -3568,21 +3576,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C135" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D135" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C135" s="1" t="inlineStr"/>
+      <c r="D135" s="3" t="inlineStr">
+        <is>
+          <t>UNKNOWN (no Node event)</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>SequenceConstruct</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B136" s="1" t="inlineStr">
@@ -3604,7 +3608,7 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>SequenceEmpty</t>
+          <t>Slice</t>
         </is>
       </c>
       <c r="B137" s="1" t="inlineStr">
@@ -3626,7 +3630,7 @@
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>SequenceErase</t>
+          <t>SoftmaxCrossEntropyLoss</t>
         </is>
       </c>
       <c r="B138" s="1" t="inlineStr">
@@ -3641,14 +3645,14 @@
       </c>
       <c r="D138" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>SequenceInsert</t>
+          <t>SpaceToDepth</t>
         </is>
       </c>
       <c r="B139" s="1" t="inlineStr">
@@ -3670,7 +3674,7 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>SequenceLength</t>
+          <t>Split</t>
         </is>
       </c>
       <c r="B140" s="1" t="inlineStr">
@@ -3692,7 +3696,7 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>SequenceMap</t>
+          <t>SplitToSequence</t>
         </is>
       </c>
       <c r="B141" s="1" t="inlineStr">
@@ -3705,16 +3709,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D141" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D141" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>Shape</t>
+          <t>Squeeze</t>
         </is>
       </c>
       <c r="B142" s="1" t="inlineStr">
@@ -3722,17 +3726,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C142" s="1" t="inlineStr"/>
-      <c r="D142" s="4" t="inlineStr">
-        <is>
-          <t>UNKNOWN (no Node event)</t>
+      <c r="C142" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D142" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>Size</t>
+          <t>StringConcat</t>
         </is>
       </c>
       <c r="B143" s="1" t="inlineStr">
@@ -3754,7 +3762,7 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>SoftmaxCrossEntropyLoss</t>
+          <t>StringNormalizer</t>
         </is>
       </c>
       <c r="B144" s="1" t="inlineStr">
@@ -3767,16 +3775,16 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="D144" s="3" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="D144" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>SpaceToDepth</t>
+          <t>StringSplit</t>
         </is>
       </c>
       <c r="B145" s="1" t="inlineStr">
@@ -3798,7 +3806,7 @@
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>SplitToSequence</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B146" s="1" t="inlineStr">
@@ -3820,7 +3828,7 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>StringConcat</t>
+          <t>Sum</t>
         </is>
       </c>
       <c r="B147" s="1" t="inlineStr">
@@ -3842,7 +3850,7 @@
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>StringNormalizer</t>
+          <t>TfIdfVectorizer</t>
         </is>
       </c>
       <c r="B148" s="1" t="inlineStr">
@@ -3864,7 +3872,7 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>StringSplit</t>
+          <t>Tile</t>
         </is>
       </c>
       <c r="B149" s="1" t="inlineStr">
@@ -3908,7 +3916,7 @@
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>Trilu</t>
+          <t>Transpose</t>
         </is>
       </c>
       <c r="B151" s="1" t="inlineStr">
@@ -3930,7 +3938,7 @@
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>Unique</t>
+          <t>Trilu</t>
         </is>
       </c>
       <c r="B152" s="1" t="inlineStr">
@@ -3952,22 +3960,2309 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="B153" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C153" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D153" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="inlineStr">
+        <is>
+          <t>Unsqueeze</t>
+        </is>
+      </c>
+      <c r="B154" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C154" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D154" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
+        <is>
           <t>Where</t>
         </is>
       </c>
-      <c r="B153" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="C153" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D153" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="B155" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C155" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D155" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="inlineStr">
+        <is>
+          <t>Xor</t>
+        </is>
+      </c>
+      <c r="B156" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C156" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D156" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Attention</t>
+        </is>
+      </c>
+      <c r="B157" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C157" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D157" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.AttnLSTM</t>
+        </is>
+      </c>
+      <c r="B158" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C158" s="1" t="inlineStr"/>
+      <c r="D158" s="4" t="inlineStr">
+        <is>
+          <t>FAIL (skipped: known crash)</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BeamSearch</t>
+        </is>
+      </c>
+      <c r="B159" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C159" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D159" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BiasAdd</t>
+        </is>
+      </c>
+      <c r="B160" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C160" s="1" t="inlineStr"/>
+      <c r="D160" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasAdd(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BiasDropout</t>
+        </is>
+      </c>
+      <c r="B161" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C161" s="1" t="inlineStr"/>
+      <c r="D161" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasDropout(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BiasGelu</t>
+        </is>
+      </c>
+      <c r="B162" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C162" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D162" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BiasSoftmax</t>
+        </is>
+      </c>
+      <c r="B163" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C163" s="1" t="inlineStr"/>
+      <c r="D163" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSoftmax(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BiasSplitGelu</t>
+        </is>
+      </c>
+      <c r="B164" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C164" s="1" t="inlineStr"/>
+      <c r="D164" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSplitGelu(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BifurcationDetector</t>
+        </is>
+      </c>
+      <c r="B165" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C165" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D165" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BitmaskBiasDropout</t>
+        </is>
+      </c>
+      <c r="B166" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C166" s="1" t="inlineStr"/>
+      <c r="D166" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskBiasDropout(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.BitmaskDropout</t>
+        </is>
+      </c>
+      <c r="B167" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C167" s="1" t="inlineStr"/>
+      <c r="D167" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskDropout(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.CDist</t>
+        </is>
+      </c>
+      <c r="B168" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C168" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D168" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.ComplexMul</t>
+        </is>
+      </c>
+      <c r="B169" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C169" s="1" t="inlineStr"/>
+      <c r="D169" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMul(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.ComplexMulConj</t>
+        </is>
+      </c>
+      <c r="B170" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C170" s="1" t="inlineStr"/>
+      <c r="D170" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMulConj(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.ConvTransposeWithDynamicPads</t>
+        </is>
+      </c>
+      <c r="B171" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C171" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D171" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.CropAndResize</t>
+        </is>
+      </c>
+      <c r="B172" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C172" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D172" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.CropAndResize</t>
+        </is>
+      </c>
+      <c r="B173" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C173" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D173" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DecoderAttention</t>
+        </is>
+      </c>
+      <c r="B174" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C174" s="1" t="inlineStr"/>
+      <c r="D174" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DecoderAttention(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DecoderMaskedMultiHeadAttention</t>
+        </is>
+      </c>
+      <c r="B175" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C175" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D175" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DecoderMaskedSelfAttention</t>
+        </is>
+      </c>
+      <c r="B176" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C176" s="1" t="inlineStr"/>
+      <c r="D176" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", com.microsoft.DecoderMaskedSelfAttention, "", -1) : ("X": tensor(float),) -&gt; ("Y": tensor(float),) , Error No Op registered for com.microsoft.DecoderMaskedSelfAttention with domain_version of 22</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DequantizeBFP</t>
+        </is>
+      </c>
+      <c r="B177" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C177" s="1" t="inlineStr"/>
+      <c r="D177" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeBFP(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DequantizeLinear</t>
+        </is>
+      </c>
+      <c r="B178" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C178" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D178" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DequantizeWithOrder</t>
+        </is>
+      </c>
+      <c r="B179" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C179" s="1" t="inlineStr"/>
+      <c r="D179" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeWithOrder(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DynamicQuantizeLSTM</t>
+        </is>
+      </c>
+      <c r="B180" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C180" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D180" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DynamicQuantizeMatMul</t>
+        </is>
+      </c>
+      <c r="B181" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C181" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D181" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.DynamicTimeWarping</t>
+        </is>
+      </c>
+      <c r="B182" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C182" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D182" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.EmbedLayerNormalization</t>
+        </is>
+      </c>
+      <c r="B183" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C183" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D183" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.ExpandDims</t>
+        </is>
+      </c>
+      <c r="B184" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C184" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D184" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.FastGelu</t>
+        </is>
+      </c>
+      <c r="B185" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C185" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D185" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.FusedConv</t>
+        </is>
+      </c>
+      <c r="B186" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C186" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D186" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.FusedGemm</t>
+        </is>
+      </c>
+      <c r="B187" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C187" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D187" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.FusedMatMul</t>
+        </is>
+      </c>
+      <c r="B188" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C188" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D188" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.FusedMatMulActivation</t>
+        </is>
+      </c>
+      <c r="B189" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C189" s="1" t="inlineStr"/>
+      <c r="D189" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GatedRelativePositionBias</t>
+        </is>
+      </c>
+      <c r="B190" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C190" s="1" t="inlineStr"/>
+      <c r="D190" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GatedRelativePositionBias(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GatherBlockQuantized</t>
+        </is>
+      </c>
+      <c r="B191" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C191" s="1" t="inlineStr"/>
+      <c r="D191" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GatherND</t>
+        </is>
+      </c>
+      <c r="B192" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C192" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D192" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Gelu</t>
+        </is>
+      </c>
+      <c r="B193" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C193" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D193" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GemmFastGelu</t>
+        </is>
+      </c>
+      <c r="B194" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C194" s="1" t="inlineStr"/>
+      <c r="D194" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFastGelu(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GemmFloat8</t>
+        </is>
+      </c>
+      <c r="B195" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C195" s="1" t="inlineStr"/>
+      <c r="D195" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFloat8(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GemmaRotaryEmbedding</t>
+        </is>
+      </c>
+      <c r="B196" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C196" s="1" t="inlineStr"/>
+      <c r="D196" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_q) of operator (GemmaRotaryEmbedding) in node () is invalid.</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GreedySearch</t>
+        </is>
+      </c>
+      <c r="B197" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C197" s="1" t="inlineStr"/>
+      <c r="D197" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GridSample</t>
+        </is>
+      </c>
+      <c r="B198" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C198" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D198" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GroupNorm</t>
+        </is>
+      </c>
+      <c r="B199" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C199" s="1" t="inlineStr"/>
+      <c r="D199" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GroupNorm(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.GroupQueryAttention</t>
+        </is>
+      </c>
+      <c r="B200" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C200" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D200" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Inverse</t>
+        </is>
+      </c>
+      <c r="B201" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C201" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D201" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Irfft</t>
+        </is>
+      </c>
+      <c r="B202" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C202" s="1" t="inlineStr"/>
+      <c r="D202" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Irfft(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.LongformerAttention</t>
+        </is>
+      </c>
+      <c r="B203" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C203" s="1" t="inlineStr"/>
+      <c r="D203" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for LongformerAttention(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MatMulBnb4</t>
+        </is>
+      </c>
+      <c r="B204" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C204" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D204" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MatMulFpQ4</t>
+        </is>
+      </c>
+      <c r="B205" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C205" s="1" t="inlineStr"/>
+      <c r="D205" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FAIL run: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Non-zero status code returned while running MatMulFpQ4 node. Name:'' Status Message: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\contrib_ops\cpu\matmul_fpq4.cc:55 onnxruntime::contrib::MatMulFpQ4::Compute buf_size &gt; 0 was false. Operator MatMulFpQ4 not yet supported on this hardware platform.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MatMulInteger16</t>
+        </is>
+      </c>
+      <c r="B206" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C206" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D206" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MatMulIntegerToFloat</t>
+        </is>
+      </c>
+      <c r="B207" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C207" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D207" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MatMulNBits</t>
+        </is>
+      </c>
+      <c r="B208" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C208" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D208" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MaxpoolWithMask</t>
+        </is>
+      </c>
+      <c r="B209" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C209" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D209" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MoE</t>
+        </is>
+      </c>
+      <c r="B210" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C210" s="1" t="inlineStr"/>
+      <c r="D210" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MoE(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MulInteger</t>
+        </is>
+      </c>
+      <c r="B211" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C211" s="1" t="inlineStr"/>
+      <c r="D211" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MulInteger(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MultiHeadAttention</t>
+        </is>
+      </c>
+      <c r="B212" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C212" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D212" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.MurmurHash3</t>
+        </is>
+      </c>
+      <c r="B213" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C213" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D213" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.NGramRepeatBlock</t>
+        </is>
+      </c>
+      <c r="B214" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C214" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D214" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.NhwcConv</t>
+        </is>
+      </c>
+      <c r="B215" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C215" s="1" t="inlineStr"/>
+      <c r="D215" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for NhwcConv(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.NhwcFusedConv</t>
+        </is>
+      </c>
+      <c r="B216" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C216" s="1" t="inlineStr"/>
+      <c r="D216" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.NhwcMaxPool</t>
+        </is>
+      </c>
+      <c r="B217" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C217" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D217" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.PackedAttention</t>
+        </is>
+      </c>
+      <c r="B218" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C218" s="1" t="inlineStr"/>
+      <c r="D218" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedAttention(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.PackedMultiHeadAttention</t>
+        </is>
+      </c>
+      <c r="B219" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C219" s="1" t="inlineStr"/>
+      <c r="D219" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedMultiHeadAttention(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Pad</t>
+        </is>
+      </c>
+      <c r="B220" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C220" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D220" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QAttention</t>
+        </is>
+      </c>
+      <c r="B221" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C221" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D221" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QGemm</t>
+        </is>
+      </c>
+      <c r="B222" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C222" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D222" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearAdd</t>
+        </is>
+      </c>
+      <c r="B223" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C223" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D223" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearAveragePool</t>
+        </is>
+      </c>
+      <c r="B224" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C224" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D224" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearConcat</t>
+        </is>
+      </c>
+      <c r="B225" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C225" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D225" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearConv</t>
+        </is>
+      </c>
+      <c r="B226" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C226" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D226" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearGlobalAveragePool</t>
+        </is>
+      </c>
+      <c r="B227" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C227" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D227" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearLeakyRelu</t>
+        </is>
+      </c>
+      <c r="B228" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C228" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D228" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearMul</t>
+        </is>
+      </c>
+      <c r="B229" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C229" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D229" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearReduceMean</t>
+        </is>
+      </c>
+      <c r="B230" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C230" s="1" t="inlineStr"/>
+      <c r="D230" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QLinearReduceMean(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearSigmoid</t>
+        </is>
+      </c>
+      <c r="B231" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C231" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D231" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearSoftmax</t>
+        </is>
+      </c>
+      <c r="B232" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C232" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D232" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QLinearWhere</t>
+        </is>
+      </c>
+      <c r="B233" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C233" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D233" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QMoE</t>
+        </is>
+      </c>
+      <c r="B234" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C234" s="1" t="inlineStr"/>
+      <c r="D234" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_input) of operator (QMoE) in node () is invalid.</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QOrderedAttention</t>
+        </is>
+      </c>
+      <c r="B235" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C235" s="1" t="inlineStr"/>
+      <c r="D235" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QOrderedGelu</t>
+        </is>
+      </c>
+      <c r="B236" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C236" s="1" t="inlineStr"/>
+      <c r="D236" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QOrderedGelu(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QOrderedLayerNormalization</t>
+        </is>
+      </c>
+      <c r="B237" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C237" s="1" t="inlineStr"/>
+      <c r="D237" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QOrderedLayerNormalization(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QOrderedLongformerAttention</t>
+        </is>
+      </c>
+      <c r="B238" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C238" s="1" t="inlineStr"/>
+      <c r="D238" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_mask) of operator (QOrderedLongformerAttention) in node () is invalid.</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QOrderedMatMul</t>
+        </is>
+      </c>
+      <c r="B239" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C239" s="1" t="inlineStr"/>
+      <c r="D239" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QuantizeBFP</t>
+        </is>
+      </c>
+      <c r="B240" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C240" s="1" t="inlineStr"/>
+      <c r="D240" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeBFP(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QuantizeLinear</t>
+        </is>
+      </c>
+      <c r="B241" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C241" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D241" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QuantizeWithOrder</t>
+        </is>
+      </c>
+      <c r="B242" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C242" s="1" t="inlineStr"/>
+      <c r="D242" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeWithOrder(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.QuickGelu</t>
+        </is>
+      </c>
+      <c r="B243" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C243" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D243" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Range</t>
+        </is>
+      </c>
+      <c r="B244" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C244" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D244" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.ReduceSumInteger</t>
+        </is>
+      </c>
+      <c r="B245" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C245" s="1" t="inlineStr"/>
+      <c r="D245" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ReduceSumInteger(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.RelativePositionBias</t>
+        </is>
+      </c>
+      <c r="B246" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C246" s="1" t="inlineStr"/>
+      <c r="D246" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RelativePositionBias(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.RemovePadding</t>
+        </is>
+      </c>
+      <c r="B247" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C247" s="1" t="inlineStr"/>
+      <c r="D247" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RemovePadding(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.RestorePadding</t>
+        </is>
+      </c>
+      <c r="B248" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C248" s="1" t="inlineStr"/>
+      <c r="D248" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RestorePadding(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Rfft</t>
+        </is>
+      </c>
+      <c r="B249" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C249" s="1" t="inlineStr"/>
+      <c r="D249" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Rfft(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.RotaryEmbedding</t>
+        </is>
+      </c>
+      <c r="B250" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C250" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D250" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.SampleOp</t>
+        </is>
+      </c>
+      <c r="B251" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C251" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D251" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Sampling</t>
+        </is>
+      </c>
+      <c r="B252" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C252" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D252" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.SkipGroupNorm</t>
+        </is>
+      </c>
+      <c r="B253" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C253" s="1" t="inlineStr"/>
+      <c r="D253" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for SkipGroupNorm(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.SkipLayerNormalization</t>
+        </is>
+      </c>
+      <c r="B254" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C254" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D254" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.SkipSimplifiedLayerNormalization</t>
+        </is>
+      </c>
+      <c r="B255" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C255" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D255" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Snpe</t>
+        </is>
+      </c>
+      <c r="B256" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C256" s="1" t="inlineStr"/>
+      <c r="D256" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Snpe(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.SparseAttention</t>
+        </is>
+      </c>
+      <c r="B257" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C257" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D257" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.SparseToDenseMatMul</t>
+        </is>
+      </c>
+      <c r="B258" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C258" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D258" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Tokenizer</t>
+        </is>
+      </c>
+      <c r="B259" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C259" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D259" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.TorchEmbedding</t>
+        </is>
+      </c>
+      <c r="B260" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C260" s="1" t="inlineStr"/>
+      <c r="D260" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for TorchEmbedding(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.TransposeMatMul</t>
+        </is>
+      </c>
+      <c r="B261" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C261" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D261" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Trilu</t>
+        </is>
+      </c>
+      <c r="B262" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C262" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D262" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.UnfoldTensor</t>
+        </is>
+      </c>
+      <c r="B263" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C263" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D263" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.Unique</t>
+        </is>
+      </c>
+      <c r="B264" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C264" s="1" t="inlineStr"/>
+      <c r="D264" s="4" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Unique(1) node with name ''</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.WhisperBeamSearch</t>
+        </is>
+      </c>
+      <c r="B265" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C265" s="1" t="inlineStr"/>
+      <c r="D265" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="inlineStr">
+        <is>
+          <t>com.microsoft.WordConvEmbedding</t>
+        </is>
+      </c>
+      <c r="B266" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="C266" s="1" t="inlineStr"/>
+      <c r="D266" s="4" t="inlineStr">
+        <is>
+          <t>FAIL (skipped: known crash)</t>
         </is>
       </c>
     </row>
@@ -3983,7 +6278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4020,10 +6315,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>142</v>
+        <v>211</v>
       </c>
       <c r="C2" t="n">
-        <v>93.40000000000001</v>
+        <v>79.59999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -4033,10 +6328,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>5.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -4075,31 +6370,57 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>1.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>NOT TESTED</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>SKIPPED</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FAIL</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>45</v>
+      </c>
+      <c r="C9" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Report generated on</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-06-05 09:44:00</t>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-06-06 17:58:28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate ONNX Node Core and Microsoft Node and improve OpenVINO/TensorRT test
</commit_message>
<xml_diff>
--- a/Execution Providers Tester/CPU/report_CPUExecutionProvider.xlsx
+++ b/Execution Providers Tester/CPU/report_CPUExecutionProvider.xlsx
@@ -41,12 +41,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DEDEDE"/>
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
+        <fgColor rgb="00DEDEDE"/>
       </patternFill>
     </fill>
     <fill>
@@ -615,7 +615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D266"/>
+  <dimension ref="A1:D263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,14 +816,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C9" s="1" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomUniformLike(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1143,7 @@
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
-      <c r="D24" s="3" t="inlineStr">
+      <c r="D24" s="4" t="inlineStr">
         <is>
           <t>UNKNOWN (no Node event)</t>
         </is>
@@ -1297,9 +1293,9 @@
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr"/>
-      <c r="D31" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DeformConv(19) node with name ''</t>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DeformConv(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -1975,7 +1971,7 @@
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
-      <c r="D62" s="4" t="inlineStr">
+      <c r="D62" s="3" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ImageDecoder(20) node with name ''</t>
         </is>
@@ -2190,14 +2186,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C72" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D72" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C72" s="1" t="inlineStr"/>
+      <c r="D72" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for LpNormalization(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2322,14 +2314,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C78" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D78" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C78" s="1" t="inlineStr"/>
+      <c r="D78" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MaxRoiPool(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2498,14 +2486,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C86" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D86" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C86" s="1" t="inlineStr"/>
+      <c r="D86" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Multinomial(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2894,14 +2878,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C104" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D104" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C104" s="1" t="inlineStr"/>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomNormal(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2916,14 +2896,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C105" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D105" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C105" s="1" t="inlineStr"/>
+      <c r="D105" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomNormalLike(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2938,14 +2914,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C106" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D106" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C106" s="1" t="inlineStr"/>
+      <c r="D106" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomUniform(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -2960,14 +2932,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C107" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D107" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C107" s="1" t="inlineStr"/>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RandomUniformLike(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -3312,14 +3280,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C123" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D123" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
+      <c r="C123" s="1" t="inlineStr"/>
+      <c r="D123" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RoiAlign(22) node with name ''</t>
         </is>
       </c>
     </row>
@@ -3577,7 +3541,7 @@
         </is>
       </c>
       <c r="C135" s="1" t="inlineStr"/>
-      <c r="D135" s="3" t="inlineStr">
+      <c r="D135" s="4" t="inlineStr">
         <is>
           <t>UNKNOWN (no Node event)</t>
         </is>
@@ -4070,7 +4034,7 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.AttnLSTM</t>
+          <t>com.microsoft.BeamSearch</t>
         </is>
       </c>
       <c r="B158" s="1" t="inlineStr">
@@ -4078,17 +4042,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C158" s="1" t="inlineStr"/>
-      <c r="D158" s="4" t="inlineStr">
-        <is>
-          <t>FAIL (skipped: known crash)</t>
+      <c r="C158" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D158" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BeamSearch</t>
+          <t>com.microsoft.BiasAdd</t>
         </is>
       </c>
       <c r="B159" s="1" t="inlineStr">
@@ -4096,21 +4064,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C159" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D159" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C159" s="1" t="inlineStr"/>
+      <c r="D159" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasAdd(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BiasAdd</t>
+          <t>com.microsoft.BiasDropout</t>
         </is>
       </c>
       <c r="B160" s="1" t="inlineStr">
@@ -4119,16 +4083,16 @@
         </is>
       </c>
       <c r="C160" s="1" t="inlineStr"/>
-      <c r="D160" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasAdd(1) node with name ''</t>
+      <c r="D160" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasDropout(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BiasDropout</t>
+          <t>com.microsoft.BiasGelu</t>
         </is>
       </c>
       <c r="B161" s="1" t="inlineStr">
@@ -4136,17 +4100,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C161" s="1" t="inlineStr"/>
-      <c r="D161" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasDropout(1) node with name ''</t>
+      <c r="C161" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D161" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BiasGelu</t>
+          <t>com.microsoft.BiasSoftmax</t>
         </is>
       </c>
       <c r="B162" s="1" t="inlineStr">
@@ -4154,21 +4122,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C162" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D162" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C162" s="1" t="inlineStr"/>
+      <c r="D162" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSoftmax(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BiasSoftmax</t>
+          <t>com.microsoft.BiasSplitGelu</t>
         </is>
       </c>
       <c r="B163" s="1" t="inlineStr">
@@ -4177,16 +4141,16 @@
         </is>
       </c>
       <c r="C163" s="1" t="inlineStr"/>
-      <c r="D163" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSoftmax(1) node with name ''</t>
+      <c r="D163" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSplitGelu(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BiasSplitGelu</t>
+          <t>com.microsoft.BifurcationDetector</t>
         </is>
       </c>
       <c r="B164" s="1" t="inlineStr">
@@ -4194,17 +4158,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C164" s="1" t="inlineStr"/>
-      <c r="D164" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BiasSplitGelu(1) node with name ''</t>
+      <c r="C164" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D164" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BifurcationDetector</t>
+          <t>com.microsoft.BitmaskBiasDropout</t>
         </is>
       </c>
       <c r="B165" s="1" t="inlineStr">
@@ -4212,21 +4180,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C165" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D165" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C165" s="1" t="inlineStr"/>
+      <c r="D165" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskBiasDropout(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BitmaskBiasDropout</t>
+          <t>com.microsoft.BitmaskDropout</t>
         </is>
       </c>
       <c r="B166" s="1" t="inlineStr">
@@ -4235,16 +4199,16 @@
         </is>
       </c>
       <c r="C166" s="1" t="inlineStr"/>
-      <c r="D166" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskBiasDropout(1) node with name ''</t>
+      <c r="D166" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskDropout(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.BitmaskDropout</t>
+          <t>com.microsoft.CDist</t>
         </is>
       </c>
       <c r="B167" s="1" t="inlineStr">
@@ -4252,17 +4216,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C167" s="1" t="inlineStr"/>
-      <c r="D167" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for BitmaskDropout(1) node with name ''</t>
+      <c r="C167" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D167" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.CDist</t>
+          <t>com.microsoft.ComplexMul</t>
         </is>
       </c>
       <c r="B168" s="1" t="inlineStr">
@@ -4270,21 +4238,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C168" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D168" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C168" s="1" t="inlineStr"/>
+      <c r="D168" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMul(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.ComplexMul</t>
+          <t>com.microsoft.ComplexMulConj</t>
         </is>
       </c>
       <c r="B169" s="1" t="inlineStr">
@@ -4293,16 +4257,16 @@
         </is>
       </c>
       <c r="C169" s="1" t="inlineStr"/>
-      <c r="D169" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMul(1) node with name ''</t>
+      <c r="D169" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMulConj(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.ComplexMulConj</t>
+          <t>com.microsoft.ConvTransposeWithDynamicPads</t>
         </is>
       </c>
       <c r="B170" s="1" t="inlineStr">
@@ -4310,17 +4274,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C170" s="1" t="inlineStr"/>
-      <c r="D170" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ComplexMulConj(1) node with name ''</t>
+      <c r="C170" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D170" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.ConvTransposeWithDynamicPads</t>
+          <t>com.microsoft.CropAndResize</t>
         </is>
       </c>
       <c r="B171" s="1" t="inlineStr">
@@ -4342,7 +4310,7 @@
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.CropAndResize</t>
+          <t>com.microsoft.DecoderAttention</t>
         </is>
       </c>
       <c r="B172" s="1" t="inlineStr">
@@ -4350,21 +4318,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C172" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D172" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C172" s="1" t="inlineStr"/>
+      <c r="D172" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DecoderAttention(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.CropAndResize</t>
+          <t>com.microsoft.DecoderMaskedMultiHeadAttention</t>
         </is>
       </c>
       <c r="B173" s="1" t="inlineStr">
@@ -4386,7 +4350,7 @@
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DecoderAttention</t>
+          <t>com.microsoft.DecoderMaskedSelfAttention</t>
         </is>
       </c>
       <c r="B174" s="1" t="inlineStr">
@@ -4395,16 +4359,16 @@
         </is>
       </c>
       <c r="C174" s="1" t="inlineStr"/>
-      <c r="D174" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DecoderAttention(1) node with name ''</t>
+      <c r="D174" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", com.microsoft.DecoderMaskedSelfAttention, "", -1) : ("X": tensor(float),) -&gt; ("Y": tensor(float),) , Error No Op registered for com.microsoft.DecoderMaskedSelfAttention with domain_version of 22</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DecoderMaskedMultiHeadAttention</t>
+          <t>com.microsoft.DequantizeBFP</t>
         </is>
       </c>
       <c r="B175" s="1" t="inlineStr">
@@ -4412,21 +4376,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C175" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D175" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C175" s="1" t="inlineStr"/>
+      <c r="D175" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeBFP(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DecoderMaskedSelfAttention</t>
+          <t>com.microsoft.DequantizeLinear</t>
         </is>
       </c>
       <c r="B176" s="1" t="inlineStr">
@@ -4434,17 +4394,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C176" s="1" t="inlineStr"/>
-      <c r="D176" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", com.microsoft.DecoderMaskedSelfAttention, "", -1) : ("X": tensor(float),) -&gt; ("Y": tensor(float),) , Error No Op registered for com.microsoft.DecoderMaskedSelfAttention with domain_version of 22</t>
+      <c r="C176" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D176" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DequantizeBFP</t>
+          <t>com.microsoft.DequantizeWithOrder</t>
         </is>
       </c>
       <c r="B177" s="1" t="inlineStr">
@@ -4453,16 +4417,16 @@
         </is>
       </c>
       <c r="C177" s="1" t="inlineStr"/>
-      <c r="D177" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeBFP(1) node with name ''</t>
+      <c r="D177" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeWithOrder(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DequantizeLinear</t>
+          <t>com.microsoft.DynamicQuantizeLSTM</t>
         </is>
       </c>
       <c r="B178" s="1" t="inlineStr">
@@ -4484,7 +4448,7 @@
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DequantizeWithOrder</t>
+          <t>com.microsoft.DynamicQuantizeMatMul</t>
         </is>
       </c>
       <c r="B179" s="1" t="inlineStr">
@@ -4492,17 +4456,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C179" s="1" t="inlineStr"/>
-      <c r="D179" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeWithOrder(1) node with name ''</t>
+      <c r="C179" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D179" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DynamicQuantizeLSTM</t>
+          <t>com.microsoft.DynamicTimeWarping</t>
         </is>
       </c>
       <c r="B180" s="1" t="inlineStr">
@@ -4524,7 +4492,7 @@
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DynamicQuantizeMatMul</t>
+          <t>com.microsoft.EmbedLayerNormalization</t>
         </is>
       </c>
       <c r="B181" s="1" t="inlineStr">
@@ -4546,7 +4514,7 @@
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.DynamicTimeWarping</t>
+          <t>com.microsoft.ExpandDims</t>
         </is>
       </c>
       <c r="B182" s="1" t="inlineStr">
@@ -4568,7 +4536,7 @@
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.EmbedLayerNormalization</t>
+          <t>com.microsoft.FastGelu</t>
         </is>
       </c>
       <c r="B183" s="1" t="inlineStr">
@@ -4590,7 +4558,7 @@
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.ExpandDims</t>
+          <t>com.microsoft.FusedConv</t>
         </is>
       </c>
       <c r="B184" s="1" t="inlineStr">
@@ -4612,7 +4580,7 @@
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.FastGelu</t>
+          <t>com.microsoft.FusedGemm</t>
         </is>
       </c>
       <c r="B185" s="1" t="inlineStr">
@@ -4634,7 +4602,7 @@
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.FusedConv</t>
+          <t>com.microsoft.FusedMatMul</t>
         </is>
       </c>
       <c r="B186" s="1" t="inlineStr">
@@ -4656,7 +4624,7 @@
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.FusedGemm</t>
+          <t>com.microsoft.FusedMatMulActivation</t>
         </is>
       </c>
       <c r="B187" s="1" t="inlineStr">
@@ -4664,21 +4632,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C187" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D187" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C187" s="1" t="inlineStr"/>
+      <c r="D187" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.FusedMatMul</t>
+          <t>com.microsoft.GatedRelativePositionBias</t>
         </is>
       </c>
       <c r="B188" s="1" t="inlineStr">
@@ -4686,21 +4650,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C188" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D188" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C188" s="1" t="inlineStr"/>
+      <c r="D188" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GatedRelativePositionBias(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.FusedMatMulActivation</t>
+          <t>com.microsoft.GatherBlockQuantized</t>
         </is>
       </c>
       <c r="B189" s="1" t="inlineStr">
@@ -4718,7 +4678,7 @@
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GatedRelativePositionBias</t>
+          <t>com.microsoft.GatherND</t>
         </is>
       </c>
       <c r="B190" s="1" t="inlineStr">
@@ -4726,17 +4686,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C190" s="1" t="inlineStr"/>
-      <c r="D190" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GatedRelativePositionBias(1) node with name ''</t>
+      <c r="C190" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D190" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GatherBlockQuantized</t>
+          <t>com.microsoft.Gelu</t>
         </is>
       </c>
       <c r="B191" s="1" t="inlineStr">
@@ -4744,17 +4708,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C191" s="1" t="inlineStr"/>
-      <c r="D191" s="5" t="inlineStr">
-        <is>
-          <t>NOT TESTED (model unavailable)</t>
+      <c r="C191" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D191" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GatherND</t>
+          <t>com.microsoft.GemmFastGelu</t>
         </is>
       </c>
       <c r="B192" s="1" t="inlineStr">
@@ -4762,21 +4730,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C192" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D192" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C192" s="1" t="inlineStr"/>
+      <c r="D192" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFastGelu(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Gelu</t>
+          <t>com.microsoft.GemmFloat8</t>
         </is>
       </c>
       <c r="B193" s="1" t="inlineStr">
@@ -4784,21 +4748,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C193" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D193" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C193" s="1" t="inlineStr"/>
+      <c r="D193" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFloat8(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GemmFastGelu</t>
+          <t>com.microsoft.GemmaRotaryEmbedding</t>
         </is>
       </c>
       <c r="B194" s="1" t="inlineStr">
@@ -4807,16 +4767,16 @@
         </is>
       </c>
       <c r="C194" s="1" t="inlineStr"/>
-      <c r="D194" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFastGelu(1) node with name ''</t>
+      <c r="D194" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_q) of operator (GemmaRotaryEmbedding) in node () is invalid.</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GemmFloat8</t>
+          <t>com.microsoft.GreedySearch</t>
         </is>
       </c>
       <c r="B195" s="1" t="inlineStr">
@@ -4825,16 +4785,16 @@
         </is>
       </c>
       <c r="C195" s="1" t="inlineStr"/>
-      <c r="D195" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFloat8(1) node with name ''</t>
+      <c r="D195" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GemmaRotaryEmbedding</t>
+          <t>com.microsoft.GridSample</t>
         </is>
       </c>
       <c r="B196" s="1" t="inlineStr">
@@ -4842,17 +4802,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C196" s="1" t="inlineStr"/>
-      <c r="D196" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_q) of operator (GemmaRotaryEmbedding) in node () is invalid.</t>
+      <c r="C196" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D196" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GreedySearch</t>
+          <t>com.microsoft.GroupNorm</t>
         </is>
       </c>
       <c r="B197" s="1" t="inlineStr">
@@ -4861,16 +4825,16 @@
         </is>
       </c>
       <c r="C197" s="1" t="inlineStr"/>
-      <c r="D197" s="5" t="inlineStr">
-        <is>
-          <t>NOT TESTED (model unavailable)</t>
+      <c r="D197" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GroupNorm(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GridSample</t>
+          <t>com.microsoft.GroupQueryAttention</t>
         </is>
       </c>
       <c r="B198" s="1" t="inlineStr">
@@ -4892,7 +4856,7 @@
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GroupNorm</t>
+          <t>com.microsoft.Inverse</t>
         </is>
       </c>
       <c r="B199" s="1" t="inlineStr">
@@ -4900,17 +4864,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C199" s="1" t="inlineStr"/>
-      <c r="D199" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GroupNorm(1) node with name ''</t>
+      <c r="C199" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D199" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.GroupQueryAttention</t>
+          <t>com.microsoft.Irfft</t>
         </is>
       </c>
       <c r="B200" s="1" t="inlineStr">
@@ -4918,21 +4886,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C200" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D200" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C200" s="1" t="inlineStr"/>
+      <c r="D200" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Irfft(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Inverse</t>
+          <t>com.microsoft.LongformerAttention</t>
         </is>
       </c>
       <c r="B201" s="1" t="inlineStr">
@@ -4940,21 +4904,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C201" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D201" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C201" s="1" t="inlineStr"/>
+      <c r="D201" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for LongformerAttention(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Irfft</t>
+          <t>com.microsoft.MatMulBnb4</t>
         </is>
       </c>
       <c r="B202" s="1" t="inlineStr">
@@ -4962,17 +4922,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C202" s="1" t="inlineStr"/>
-      <c r="D202" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Irfft(1) node with name ''</t>
+      <c r="C202" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D202" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.LongformerAttention</t>
+          <t>com.microsoft.MatMulFpQ4</t>
         </is>
       </c>
       <c r="B203" s="1" t="inlineStr">
@@ -4981,16 +4945,17 @@
         </is>
       </c>
       <c r="C203" s="1" t="inlineStr"/>
-      <c r="D203" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for LongformerAttention(1) node with name ''</t>
+      <c r="D203" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FAIL run: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Non-zero status code returned while running MatMulFpQ4 node. Name:'' Status Message: C:\Users\COCO\onnxruntime_1_22_test\onnxruntime\contrib_ops\cpu\matmul_fpq4.cc:55 onnxruntime::contrib::MatMulFpQ4::Compute buf_size &gt; 0 was false. Operator MatMulFpQ4 not yet supported on this hardware platform.
+</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MatMulBnb4</t>
+          <t>com.microsoft.MatMulInteger16</t>
         </is>
       </c>
       <c r="B204" s="1" t="inlineStr">
@@ -5012,7 +4977,7 @@
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MatMulFpQ4</t>
+          <t>com.microsoft.MatMulIntegerToFloat</t>
         </is>
       </c>
       <c r="B205" s="1" t="inlineStr">
@@ -5020,18 +4985,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C205" s="1" t="inlineStr"/>
-      <c r="D205" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FAIL run: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Non-zero status code returned while running MatMulFpQ4 node. Name:'' Status Message: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\contrib_ops\cpu\matmul_fpq4.cc:55 onnxruntime::contrib::MatMulFpQ4::Compute buf_size &gt; 0 was false. Operator MatMulFpQ4 not yet supported on this hardware platform.
-</t>
+      <c r="C205" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D205" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MatMulInteger16</t>
+          <t>com.microsoft.MatMulNBits</t>
         </is>
       </c>
       <c r="B206" s="1" t="inlineStr">
@@ -5053,7 +5021,7 @@
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MatMulIntegerToFloat</t>
+          <t>com.microsoft.MaxpoolWithMask</t>
         </is>
       </c>
       <c r="B207" s="1" t="inlineStr">
@@ -5075,7 +5043,7 @@
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MatMulNBits</t>
+          <t>com.microsoft.MoE</t>
         </is>
       </c>
       <c r="B208" s="1" t="inlineStr">
@@ -5083,21 +5051,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C208" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D208" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C208" s="1" t="inlineStr"/>
+      <c r="D208" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MoE(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MaxpoolWithMask</t>
+          <t>com.microsoft.MulInteger</t>
         </is>
       </c>
       <c r="B209" s="1" t="inlineStr">
@@ -5105,21 +5069,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C209" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D209" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C209" s="1" t="inlineStr"/>
+      <c r="D209" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MulInteger(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MoE</t>
+          <t>com.microsoft.MultiHeadAttention</t>
         </is>
       </c>
       <c r="B210" s="1" t="inlineStr">
@@ -5127,17 +5087,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C210" s="1" t="inlineStr"/>
-      <c r="D210" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MoE(1) node with name ''</t>
+      <c r="C210" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D210" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MulInteger</t>
+          <t>com.microsoft.MurmurHash3</t>
         </is>
       </c>
       <c r="B211" s="1" t="inlineStr">
@@ -5145,17 +5109,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C211" s="1" t="inlineStr"/>
-      <c r="D211" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MulInteger(1) node with name ''</t>
+      <c r="C211" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D211" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MultiHeadAttention</t>
+          <t>com.microsoft.NGramRepeatBlock</t>
         </is>
       </c>
       <c r="B212" s="1" t="inlineStr">
@@ -5177,7 +5145,7 @@
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.MurmurHash3</t>
+          <t>com.microsoft.NhwcConv</t>
         </is>
       </c>
       <c r="B213" s="1" t="inlineStr">
@@ -5185,21 +5153,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C213" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D213" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C213" s="1" t="inlineStr"/>
+      <c r="D213" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for NhwcConv(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.NGramRepeatBlock</t>
+          <t>com.microsoft.NhwcFusedConv</t>
         </is>
       </c>
       <c r="B214" s="1" t="inlineStr">
@@ -5207,21 +5171,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C214" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D214" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C214" s="1" t="inlineStr"/>
+      <c r="D214" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.NhwcConv</t>
+          <t>com.microsoft.NhwcMaxPool</t>
         </is>
       </c>
       <c r="B215" s="1" t="inlineStr">
@@ -5229,17 +5189,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C215" s="1" t="inlineStr"/>
-      <c r="D215" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for NhwcConv(1) node with name ''</t>
+      <c r="C215" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D215" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.NhwcFusedConv</t>
+          <t>com.microsoft.PackedAttention</t>
         </is>
       </c>
       <c r="B216" s="1" t="inlineStr">
@@ -5248,16 +5212,16 @@
         </is>
       </c>
       <c r="C216" s="1" t="inlineStr"/>
-      <c r="D216" s="5" t="inlineStr">
-        <is>
-          <t>NOT TESTED (model unavailable)</t>
+      <c r="D216" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedAttention(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.NhwcMaxPool</t>
+          <t>com.microsoft.PackedMultiHeadAttention</t>
         </is>
       </c>
       <c r="B217" s="1" t="inlineStr">
@@ -5265,21 +5229,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C217" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D217" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C217" s="1" t="inlineStr"/>
+      <c r="D217" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedMultiHeadAttention(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.PackedAttention</t>
+          <t>com.microsoft.Pad</t>
         </is>
       </c>
       <c r="B218" s="1" t="inlineStr">
@@ -5287,17 +5247,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C218" s="1" t="inlineStr"/>
-      <c r="D218" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedAttention(1) node with name ''</t>
+      <c r="C218" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D218" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.PackedMultiHeadAttention</t>
+          <t>com.microsoft.QAttention</t>
         </is>
       </c>
       <c r="B219" s="1" t="inlineStr">
@@ -5305,17 +5269,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C219" s="1" t="inlineStr"/>
-      <c r="D219" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for PackedMultiHeadAttention(1) node with name ''</t>
+      <c r="C219" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D219" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Pad</t>
+          <t>com.microsoft.QGemm</t>
         </is>
       </c>
       <c r="B220" s="1" t="inlineStr">
@@ -5337,7 +5305,7 @@
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QAttention</t>
+          <t>com.microsoft.QLinearAdd</t>
         </is>
       </c>
       <c r="B221" s="1" t="inlineStr">
@@ -5359,7 +5327,7 @@
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QGemm</t>
+          <t>com.microsoft.QLinearAveragePool</t>
         </is>
       </c>
       <c r="B222" s="1" t="inlineStr">
@@ -5381,7 +5349,7 @@
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearAdd</t>
+          <t>com.microsoft.QLinearConcat</t>
         </is>
       </c>
       <c r="B223" s="1" t="inlineStr">
@@ -5403,7 +5371,7 @@
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearAveragePool</t>
+          <t>com.microsoft.QLinearConv</t>
         </is>
       </c>
       <c r="B224" s="1" t="inlineStr">
@@ -5425,7 +5393,7 @@
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearConcat</t>
+          <t>com.microsoft.QLinearGlobalAveragePool</t>
         </is>
       </c>
       <c r="B225" s="1" t="inlineStr">
@@ -5447,7 +5415,7 @@
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearConv</t>
+          <t>com.microsoft.QLinearLeakyRelu</t>
         </is>
       </c>
       <c r="B226" s="1" t="inlineStr">
@@ -5469,7 +5437,7 @@
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearGlobalAveragePool</t>
+          <t>com.microsoft.QLinearMul</t>
         </is>
       </c>
       <c r="B227" s="1" t="inlineStr">
@@ -5491,7 +5459,7 @@
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearLeakyRelu</t>
+          <t>com.microsoft.QLinearReduceMean</t>
         </is>
       </c>
       <c r="B228" s="1" t="inlineStr">
@@ -5499,21 +5467,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C228" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D228" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C228" s="1" t="inlineStr"/>
+      <c r="D228" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QLinearReduceMean(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearMul</t>
+          <t>com.microsoft.QLinearSigmoid</t>
         </is>
       </c>
       <c r="B229" s="1" t="inlineStr">
@@ -5535,7 +5499,7 @@
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearReduceMean</t>
+          <t>com.microsoft.QLinearSoftmax</t>
         </is>
       </c>
       <c r="B230" s="1" t="inlineStr">
@@ -5543,17 +5507,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C230" s="1" t="inlineStr"/>
-      <c r="D230" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QLinearReduceMean(1) node with name ''</t>
+      <c r="C230" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D230" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearSigmoid</t>
+          <t>com.microsoft.QLinearWhere</t>
         </is>
       </c>
       <c r="B231" s="1" t="inlineStr">
@@ -5575,7 +5543,7 @@
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearSoftmax</t>
+          <t>com.microsoft.QMoE</t>
         </is>
       </c>
       <c r="B232" s="1" t="inlineStr">
@@ -5583,21 +5551,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C232" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D232" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C232" s="1" t="inlineStr"/>
+      <c r="D232" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_input) of operator (QMoE) in node () is invalid.</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QLinearWhere</t>
+          <t>com.microsoft.QOrderedAttention</t>
         </is>
       </c>
       <c r="B233" s="1" t="inlineStr">
@@ -5605,21 +5569,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C233" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D233" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C233" s="1" t="inlineStr"/>
+      <c r="D233" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QMoE</t>
+          <t>com.microsoft.QOrderedGelu</t>
         </is>
       </c>
       <c r="B234" s="1" t="inlineStr">
@@ -5628,16 +5588,16 @@
         </is>
       </c>
       <c r="C234" s="1" t="inlineStr"/>
-      <c r="D234" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_input) of operator (QMoE) in node () is invalid.</t>
+      <c r="D234" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QOrderedGelu(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QOrderedAttention</t>
+          <t>com.microsoft.QOrderedLayerNormalization</t>
         </is>
       </c>
       <c r="B235" s="1" t="inlineStr">
@@ -5646,16 +5606,16 @@
         </is>
       </c>
       <c r="C235" s="1" t="inlineStr"/>
-      <c r="D235" s="5" t="inlineStr">
-        <is>
-          <t>NOT TESTED (model unavailable)</t>
+      <c r="D235" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QOrderedLayerNormalization(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QOrderedGelu</t>
+          <t>com.microsoft.QOrderedLongformerAttention</t>
         </is>
       </c>
       <c r="B236" s="1" t="inlineStr">
@@ -5664,16 +5624,16 @@
         </is>
       </c>
       <c r="C236" s="1" t="inlineStr"/>
-      <c r="D236" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QOrderedGelu(1) node with name ''</t>
+      <c r="D236" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_mask) of operator (QOrderedLongformerAttention) in node () is invalid.</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QOrderedLayerNormalization</t>
+          <t>com.microsoft.QOrderedMatMul</t>
         </is>
       </c>
       <c r="B237" s="1" t="inlineStr">
@@ -5682,16 +5642,16 @@
         </is>
       </c>
       <c r="C237" s="1" t="inlineStr"/>
-      <c r="D237" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QOrderedLayerNormalization(1) node with name ''</t>
+      <c r="D237" s="5" t="inlineStr">
+        <is>
+          <t>NOT TESTED (model unavailable)</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QOrderedLongformerAttention</t>
+          <t>com.microsoft.QuantizeBFP</t>
         </is>
       </c>
       <c r="B238" s="1" t="inlineStr">
@@ -5700,16 +5660,16 @@
         </is>
       </c>
       <c r="C238" s="1" t="inlineStr"/>
-      <c r="D238" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. Type Error: Type 'tensor(float)' of input parameter (InsertedPrecisionFreeCast_mask) of operator (QOrderedLongformerAttention) in node () is invalid.</t>
+      <c r="D238" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeBFP(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QOrderedMatMul</t>
+          <t>com.microsoft.QuantizeLinear</t>
         </is>
       </c>
       <c r="B239" s="1" t="inlineStr">
@@ -5717,17 +5677,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C239" s="1" t="inlineStr"/>
-      <c r="D239" s="5" t="inlineStr">
-        <is>
-          <t>NOT TESTED (model unavailable)</t>
+      <c r="C239" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D239" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QuantizeBFP</t>
+          <t>com.microsoft.QuantizeWithOrder</t>
         </is>
       </c>
       <c r="B240" s="1" t="inlineStr">
@@ -5736,16 +5700,16 @@
         </is>
       </c>
       <c r="C240" s="1" t="inlineStr"/>
-      <c r="D240" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeBFP(1) node with name ''</t>
+      <c r="D240" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeWithOrder(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QuantizeLinear</t>
+          <t>com.microsoft.QuickGelu</t>
         </is>
       </c>
       <c r="B241" s="1" t="inlineStr">
@@ -5767,7 +5731,7 @@
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QuantizeWithOrder</t>
+          <t>com.microsoft.Range</t>
         </is>
       </c>
       <c r="B242" s="1" t="inlineStr">
@@ -5775,17 +5739,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C242" s="1" t="inlineStr"/>
-      <c r="D242" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeWithOrder(1) node with name ''</t>
+      <c r="C242" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D242" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.QuickGelu</t>
+          <t>com.microsoft.ReduceSumInteger</t>
         </is>
       </c>
       <c r="B243" s="1" t="inlineStr">
@@ -5793,21 +5761,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C243" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D243" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C243" s="1" t="inlineStr"/>
+      <c r="D243" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ReduceSumInteger(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Range</t>
+          <t>com.microsoft.RelativePositionBias</t>
         </is>
       </c>
       <c r="B244" s="1" t="inlineStr">
@@ -5815,21 +5779,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C244" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D244" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C244" s="1" t="inlineStr"/>
+      <c r="D244" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RelativePositionBias(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.ReduceSumInteger</t>
+          <t>com.microsoft.RemovePadding</t>
         </is>
       </c>
       <c r="B245" s="1" t="inlineStr">
@@ -5838,16 +5798,16 @@
         </is>
       </c>
       <c r="C245" s="1" t="inlineStr"/>
-      <c r="D245" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ReduceSumInteger(1) node with name ''</t>
+      <c r="D245" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RemovePadding(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.RelativePositionBias</t>
+          <t>com.microsoft.RestorePadding</t>
         </is>
       </c>
       <c r="B246" s="1" t="inlineStr">
@@ -5856,16 +5816,16 @@
         </is>
       </c>
       <c r="C246" s="1" t="inlineStr"/>
-      <c r="D246" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RelativePositionBias(1) node with name ''</t>
+      <c r="D246" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RestorePadding(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.RemovePadding</t>
+          <t>com.microsoft.Rfft</t>
         </is>
       </c>
       <c r="B247" s="1" t="inlineStr">
@@ -5874,16 +5834,16 @@
         </is>
       </c>
       <c r="C247" s="1" t="inlineStr"/>
-      <c r="D247" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RemovePadding(1) node with name ''</t>
+      <c r="D247" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Rfft(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.RestorePadding</t>
+          <t>com.microsoft.RotaryEmbedding</t>
         </is>
       </c>
       <c r="B248" s="1" t="inlineStr">
@@ -5891,17 +5851,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C248" s="1" t="inlineStr"/>
-      <c r="D248" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for RestorePadding(1) node with name ''</t>
+      <c r="C248" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D248" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Rfft</t>
+          <t>com.microsoft.SampleOp</t>
         </is>
       </c>
       <c r="B249" s="1" t="inlineStr">
@@ -5909,17 +5873,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C249" s="1" t="inlineStr"/>
-      <c r="D249" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Rfft(1) node with name ''</t>
+      <c r="C249" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D249" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.RotaryEmbedding</t>
+          <t>com.microsoft.Sampling</t>
         </is>
       </c>
       <c r="B250" s="1" t="inlineStr">
@@ -5941,7 +5909,7 @@
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.SampleOp</t>
+          <t>com.microsoft.SkipGroupNorm</t>
         </is>
       </c>
       <c r="B251" s="1" t="inlineStr">
@@ -5949,21 +5917,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C251" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D251" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C251" s="1" t="inlineStr"/>
+      <c r="D251" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for SkipGroupNorm(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Sampling</t>
+          <t>com.microsoft.SkipLayerNormalization</t>
         </is>
       </c>
       <c r="B252" s="1" t="inlineStr">
@@ -5985,7 +5949,7 @@
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.SkipGroupNorm</t>
+          <t>com.microsoft.SkipSimplifiedLayerNormalization</t>
         </is>
       </c>
       <c r="B253" s="1" t="inlineStr">
@@ -5993,17 +5957,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C253" s="1" t="inlineStr"/>
-      <c r="D253" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for SkipGroupNorm(1) node with name ''</t>
+      <c r="C253" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D253" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.SkipLayerNormalization</t>
+          <t>com.microsoft.Snpe</t>
         </is>
       </c>
       <c r="B254" s="1" t="inlineStr">
@@ -6011,21 +5979,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C254" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D254" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C254" s="1" t="inlineStr"/>
+      <c r="D254" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Snpe(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.SkipSimplifiedLayerNormalization</t>
+          <t>com.microsoft.SparseAttention</t>
         </is>
       </c>
       <c r="B255" s="1" t="inlineStr">
@@ -6047,7 +6011,7 @@
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Snpe</t>
+          <t>com.microsoft.SparseToDenseMatMul</t>
         </is>
       </c>
       <c r="B256" s="1" t="inlineStr">
@@ -6055,17 +6019,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C256" s="1" t="inlineStr"/>
-      <c r="D256" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Snpe(1) node with name ''</t>
+      <c r="C256" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D256" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.SparseAttention</t>
+          <t>com.microsoft.Tokenizer</t>
         </is>
       </c>
       <c r="B257" s="1" t="inlineStr">
@@ -6087,7 +6055,7 @@
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.SparseToDenseMatMul</t>
+          <t>com.microsoft.TorchEmbedding</t>
         </is>
       </c>
       <c r="B258" s="1" t="inlineStr">
@@ -6095,21 +6063,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C258" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D258" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C258" s="1" t="inlineStr"/>
+      <c r="D258" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for TorchEmbedding(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Tokenizer</t>
+          <t>com.microsoft.TransposeMatMul</t>
         </is>
       </c>
       <c r="B259" s="1" t="inlineStr">
@@ -6131,7 +6095,7 @@
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.TorchEmbedding</t>
+          <t>com.microsoft.Trilu</t>
         </is>
       </c>
       <c r="B260" s="1" t="inlineStr">
@@ -6139,17 +6103,21 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C260" s="1" t="inlineStr"/>
-      <c r="D260" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for TorchEmbedding(1) node with name ''</t>
+      <c r="C260" s="1" t="inlineStr">
+        <is>
+          <t>CPUExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D260" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.TransposeMatMul</t>
+          <t>com.microsoft.UnfoldTensor</t>
         </is>
       </c>
       <c r="B261" s="1" t="inlineStr">
@@ -6171,7 +6139,7 @@
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.Trilu</t>
+          <t>com.microsoft.Unique</t>
         </is>
       </c>
       <c r="B262" s="1" t="inlineStr">
@@ -6179,21 +6147,17 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C262" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D262" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
+      <c r="C262" s="1" t="inlineStr"/>
+      <c r="D262" s="3" t="inlineStr">
+        <is>
+          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Unique(1) node with name ''</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>com.microsoft.UnfoldTensor</t>
+          <t>com.microsoft.WhisperBeamSearch</t>
         </is>
       </c>
       <c r="B263" s="1" t="inlineStr">
@@ -6201,68 +6165,10 @@
           <t>CPUExecutionProvider</t>
         </is>
       </c>
-      <c r="C263" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="D263" s="2" t="inlineStr">
-        <is>
-          <t>SUCCESS (via decomposition)</t>
-        </is>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" s="1" t="inlineStr">
-        <is>
-          <t>com.microsoft.Unique</t>
-        </is>
-      </c>
-      <c r="B264" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="C264" s="1" t="inlineStr"/>
-      <c r="D264" s="4" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Unique(1) node with name ''</t>
-        </is>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" s="1" t="inlineStr">
-        <is>
-          <t>com.microsoft.WhisperBeamSearch</t>
-        </is>
-      </c>
-      <c r="B265" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="C265" s="1" t="inlineStr"/>
-      <c r="D265" s="5" t="inlineStr">
+      <c r="C263" s="1" t="inlineStr"/>
+      <c r="D263" s="5" t="inlineStr">
         <is>
           <t>NOT TESTED (model unavailable)</t>
-        </is>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" s="1" t="inlineStr">
-        <is>
-          <t>com.microsoft.WordConvEmbedding</t>
-        </is>
-      </c>
-      <c r="B266" s="1" t="inlineStr">
-        <is>
-          <t>CPUExecutionProvider</t>
-        </is>
-      </c>
-      <c r="C266" s="1" t="inlineStr"/>
-      <c r="D266" s="4" t="inlineStr">
-        <is>
-          <t>FAIL (skipped: known crash)</t>
         </is>
       </c>
     </row>
@@ -6315,10 +6221,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C2" t="n">
-        <v>79.59999999999999</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="3">
@@ -6383,7 +6289,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="8">
@@ -6406,10 +6312,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>19.8</v>
       </c>
     </row>
     <row r="10">
@@ -6420,7 +6326,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-06-06 17:58:28</t>
+          <t>2025-07-11 10:42:58</t>
         </is>
       </c>
     </row>

</xml_diff>